<commit_message>
added separate functions for creating sample data
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/DistanceCalculationReverse.xlsx
+++ b/pyloghub/sample_data/DistanceCalculationReverse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5D5404-720A-4D53-ACFE-99B9BF9B8BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791F7C82-6606-4420-B2DF-ACE97F4D2493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7A75092-82F1-48BA-B51D-2D37F8097956}"/>
   </bookViews>
@@ -135,6 +135,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,9 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,12 +532,13 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -560,7 +565,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>37.779280800000002</v>
       </c>
       <c r="C2">
@@ -580,7 +585,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>37.779280800000002</v>
       </c>
       <c r="C3">

</xml_diff>